<commit_message>
add the field dosage
</commit_message>
<xml_diff>
--- a/doc/Diccionario.xlsx
+++ b/doc/Diccionario.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="65">
   <si>
     <t xml:space="preserve">PLANTILLA DE DICCIONARIO DE DATOS</t>
   </si>
@@ -177,6 +177,12 @@
     <t xml:space="preserve">integer</t>
   </si>
   <si>
+    <t xml:space="preserve">integerMaxValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
     <t xml:space="preserve">NO</t>
   </si>
   <si>
@@ -204,6 +210,9 @@
     <t xml:space="preserve">Alfanumerico y caracteres especiales</t>
   </si>
   <si>
+    <t xml:space="preserve">Concentración </t>
+  </si>
+  <si>
     <t xml:space="preserve">Brand</t>
   </si>
   <si>
@@ -217,6 +226,9 @@
   </si>
   <si>
     <t xml:space="preserve">real</t>
+  </si>
+  <si>
+    <t xml:space="preserve">real max Value</t>
   </si>
   <si>
     <t xml:space="preserve">Stock</t>
@@ -594,9 +606,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>885600</xdr:colOff>
+      <xdr:colOff>885240</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>537480</xdr:rowOff>
+      <xdr:rowOff>537120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -609,8 +621,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2552760" y="676080"/>
-          <a:ext cx="475920" cy="404280"/>
+          <a:off x="2533680" y="676080"/>
+          <a:ext cx="475560" cy="403920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -636,9 +648,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1152000</xdr:colOff>
+      <xdr:colOff>1151640</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>430920</xdr:rowOff>
+      <xdr:rowOff>430560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -651,8 +663,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2266560" y="647640"/>
-          <a:ext cx="313920" cy="326160"/>
+          <a:off x="2247480" y="647640"/>
+          <a:ext cx="313560" cy="325800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -678,9 +690,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>302400</xdr:colOff>
+      <xdr:colOff>302040</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>411120</xdr:rowOff>
+      <xdr:rowOff>410760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -693,8 +705,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5804280" y="654840"/>
-          <a:ext cx="582480" cy="299160"/>
+          <a:off x="5730120" y="654840"/>
+          <a:ext cx="563040" cy="298800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -724,12 +736,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="30.3724489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="49.2704081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="32.3979591836735"/>
-    <col collapsed="false" hidden="false" max="9" min="4" style="1" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="48.7295918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.9948979591837"/>
+    <col collapsed="false" hidden="false" max="9" min="4" style="1" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -847,12 +859,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="20.25"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="8" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="8" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -969,6 +981,13 @@
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
+    </row>
+    <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0"/>
+      <c r="B14" s="0"/>
+      <c r="C14" s="0"/>
+      <c r="D14" s="0"/>
+      <c r="E14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
@@ -1001,30 +1020,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="bottomRight" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="30.0765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="8" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="8" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="8" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="8" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="8" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="8" width="14.7142857142857"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="8" width="38.25"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="8" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="8" width="23.6938775510204"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="8" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="8" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="8" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="8" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="8" width="37.7959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1154,115 +1173,151 @@
       <c r="E6" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
+      <c r="F6" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>42</v>
+      </c>
       <c r="H6" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
+        <v>43</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>43</v>
+      </c>
       <c r="K6" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11"/>
       <c r="B7" s="12" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
+        <v>47</v>
+      </c>
+      <c r="F7" s="12" t="n">
+        <v>100</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>42</v>
+      </c>
       <c r="H7" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
+        <v>43</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>43</v>
+      </c>
       <c r="K7" s="12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11"/>
       <c r="B8" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
+      <c r="F8" s="12" t="n">
+        <v>255</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>42</v>
+      </c>
       <c r="H8" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
+        <v>43</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>43</v>
+      </c>
       <c r="K8" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11"/>
-      <c r="B9" s="12" t="s">
-        <v>50</v>
-      </c>
+      <c r="B9" s="12"/>
       <c r="C9" s="12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
+        <v>47</v>
+      </c>
+      <c r="F9" s="12" t="n">
+        <v>100</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>42</v>
+      </c>
       <c r="H9" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12" t="s">
-        <v>49</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" s="12"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11"/>
       <c r="B10" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
+        <v>47</v>
+      </c>
+      <c r="F10" s="12" t="n">
+        <v>100</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>42</v>
+      </c>
       <c r="H10" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="15" t="n">
-        <v>0</v>
+        <v>43</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1274,81 +1329,130 @@
         <v>56</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
+        <v>57</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>42</v>
+      </c>
       <c r="H11" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12" t="s">
-        <v>57</v>
+        <v>43</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="K11" s="15" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11"/>
       <c r="B12" s="12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D12" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
+      <c r="G12" s="12" t="s">
+        <v>42</v>
+      </c>
       <c r="H12" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
+        <v>43</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>43</v>
+      </c>
       <c r="K12" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-    </row>
-    <row r="14" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="11"/>
+      <c r="B13" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="12" t="n">
+        <v>255</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+    </row>
+    <row r="15" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A5:A12"/>
-    <mergeCell ref="A14:K14"/>
+    <mergeCell ref="A5:A13"/>
+    <mergeCell ref="A15:K15"/>
   </mergeCells>
   <conditionalFormatting sqref="D1">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">

</xml_diff>